<commit_message>
t11.1 - correção de filtragem da tabela do siconfi
</commit_message>
<xml_diff>
--- a/Data/t11.1.xlsx
+++ b/Data/t11.1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1051,25 +1051,25 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Receitas Tributárias</t>
+          <t>Receitas de Exploração de Recursos Naturais</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Total (1)</t>
+          <t>Total (3)</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>-99.99920705429672</v>
+        <v>-1.121216821977611</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1082,12 +1082,12 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>-1.121216821977611</v>
+        <v>-46.817824810541</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1100,12 +1100,12 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-46.817824810541</v>
+        <v>-31.44547510309983</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1118,12 +1118,12 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>-31.44547510309983</v>
+        <v>-2.948205694391848</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1136,12 +1136,12 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>-2.948205694391848</v>
+        <v>15.01771256682733</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1154,12 +1154,12 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>15.01771256682733</v>
+        <v>-20.03643175044765</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1172,12 +1172,12 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>-20.03643175044765</v>
+        <v>-20.67228986991331</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1190,12 +1190,12 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>-20.67228986991331</v>
+        <v>11.91783576722245</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1208,12 +1208,12 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>11.91783576722245</v>
+        <v>44.82592946317314</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1226,12 +1226,12 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>44.82592946317314</v>
+        <v>-35.87025361669786</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1244,30 +1244,30 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>-35.87025361669786</v>
+        <v>26.44573759185258</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Receitas de Exploração de Recursos Naturais</t>
+          <t>Transferências Federais</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Total (3)</t>
+          <t>Fundeb</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>26.44573759185258</v>
+        <v>-1.050745985120649</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1280,12 +1280,12 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>-1.050745985120649</v>
+        <v>-7.493146079046776</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1298,12 +1298,12 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>-7.493146079046776</v>
+        <v>1.677754082062677</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1316,12 +1316,12 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1.677754082062677</v>
+        <v>-3.335791029940871</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1334,12 +1334,12 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>-3.335791029940871</v>
+        <v>5.808699603470968</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1352,12 +1352,12 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>5.808699603470968</v>
+        <v>-1.74237194029041</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1370,12 +1370,12 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>-1.74237194029041</v>
+        <v>-7.79704214867224</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1388,12 +1388,12 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>-7.79704214867224</v>
+        <v>17.82952282634764</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1406,12 +1406,12 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>17.82952282634764</v>
+        <v>14.13996924257421</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1424,12 +1424,12 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>14.13996924257421</v>
+        <v>3.254075410574742</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1442,12 +1442,12 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>3.254075410574742</v>
+        <v>3.251088949624781</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1456,16 +1456,16 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Fundeb</t>
+          <t>Fundo de Participação dos Estados</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>3.251088949624781</v>
+        <v>2.409290835890476</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1478,12 +1478,12 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>2.409290835890476</v>
+        <v>-4.946685733405854</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1496,12 +1496,12 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>-4.946685733405854</v>
+        <v>5.961975945722298</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1514,12 +1514,12 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>5.961975945722298</v>
+        <v>-6.389518142136009</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1532,12 +1532,12 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>-6.389518142136009</v>
+        <v>2.762736106076624</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1550,12 +1550,12 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>2.762736106076624</v>
+        <v>4.889695411025086</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -1568,12 +1568,12 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>4.889695411025086</v>
+        <v>-8.527616269027838</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -1586,12 +1586,12 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>-8.527616269027838</v>
+        <v>20.7066685806667</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1604,12 +1604,12 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20.7066685806667</v>
+        <v>14.95317686156681</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1622,12 +1622,12 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>14.95317686156681</v>
+        <v>0.5246649380495905</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -1640,12 +1640,12 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.5246649380495905</v>
+        <v>9.330859627920308</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1654,16 +1654,16 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Fundo de Participação dos Estados</t>
+          <t>Total (2)</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>9.330859627920308</v>
+        <v>0.3913311029190458</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -1676,12 +1676,12 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.3913311029190458</v>
+        <v>-7.525355182452831</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -1694,12 +1694,12 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>-7.525355182452831</v>
+        <v>4.714949766020449</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -1712,12 +1712,12 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>4.714949766020449</v>
+        <v>-4.934173426721832</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -1730,12 +1730,12 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>-4.934173426721832</v>
+        <v>5.774829641842771</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -1748,12 +1748,12 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>-98.9481203945152</v>
+        <v>5.802324679288562</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -1766,12 +1766,12 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>9955.792420568079</v>
+        <v>7.581511795768359</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -1784,12 +1784,12 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>-98.79365103458146</v>
+        <v>-1.876111608518882</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -1802,12 +1802,12 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>8670.457613198299</v>
+        <v>13.31183179031803</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -1820,12 +1820,12 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>-98.46865034184459</v>
+        <v>4.645733788933248</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -1838,169 +1838,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>6925.274157526867</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D79" t="n">
-        <v>-97.18736289744623</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D80" t="n">
-        <v>3388.679300375744</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>-97.66881328225352</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D82" t="n">
-        <v>4760.693093681293</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D83" t="n">
-        <v>-98.6618780377533</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>2023</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D84" t="n">
-        <v>7720.343491951493</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>2023</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D85" t="n">
-        <v>-98.66184485220973</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>2024</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D86" t="n">
-        <v>8067.233757974019</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>2024</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Transferências Federais</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Total (2)</t>
-        </is>
-      </c>
-      <c r="D87" t="n">
-        <v>-98.55073716732846</v>
+        <v>9.290258964394194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>